<commit_message>
register.json data mapped on page
</commit_message>
<xml_diff>
--- a/data/excel/register.xlsx
+++ b/data/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BB189E-ACB8-4F97-ACB2-198AB57498B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FED0C29-2D06-47CE-8926-C50ADE7E2DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{976B87C4-C0CE-403F-B874-A2541471D161}"/>
   </bookViews>
@@ -51,18 +51,12 @@
     <t>table tennis</t>
   </si>
   <si>
-    <t>Duo/Team</t>
-  </si>
-  <si>
     <t>College Name</t>
   </si>
   <si>
     <t>Contact Number</t>
   </si>
   <si>
-    <t xml:space="preserve"> Screenshot of Payment </t>
-  </si>
-  <si>
     <t>Full Name</t>
   </si>
   <si>
@@ -82,6 +76,12 @@
   </si>
   <si>
     <t>Player</t>
+  </si>
+  <si>
+    <t>Duo</t>
+  </si>
+  <si>
+    <t>Screenshot of Payment</t>
   </si>
 </sst>
 </file>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D5B469-0A3B-4C52-9B00-630143401BDD}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,40 +454,40 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Google Form connection try
</commit_message>
<xml_diff>
--- a/data/excel/register.xlsx
+++ b/data/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FED0C29-2D06-47CE-8926-C50ADE7E2DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDBB663-EA6B-4609-BFB8-184E6099DE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{976B87C4-C0CE-403F-B874-A2541471D161}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Team Name</t>
   </si>
@@ -82,19 +82,54 @@
   </si>
   <si>
     <t>Screenshot of Payment</t>
+  </si>
+  <si>
+    <t>SportsName</t>
+  </si>
+  <si>
+    <t>entry.2092238618</t>
+  </si>
+  <si>
+    <t>entry.1556369182</t>
+  </si>
+  <si>
+    <t>entry.479301265</t>
+  </si>
+  <si>
+    <t>entry.1753222212</t>
+  </si>
+  <si>
+    <t>entry.588393791</t>
+  </si>
+  <si>
+    <t>entry.831172357</t>
+  </si>
+  <si>
+    <t>entry.2109138769</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,8 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +473,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,331 +486,335 @@
     <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
         <v>7</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>11</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>5</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Google Form connection success without image
</commit_message>
<xml_diff>
--- a/data/excel/register.xlsx
+++ b/data/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDBB663-EA6B-4609-BFB8-184E6099DE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924BE672-8E2F-493C-ADCF-9F040C0DDE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{976B87C4-C0CE-403F-B874-A2541471D161}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Team Name</t>
   </si>
@@ -87,49 +87,35 @@
     <t>SportsName</t>
   </si>
   <si>
-    <t>entry.2092238618</t>
-  </si>
-  <si>
-    <t>entry.1556369182</t>
-  </si>
-  <si>
-    <t>entry.479301265</t>
-  </si>
-  <si>
-    <t>entry.1753222212</t>
-  </si>
-  <si>
-    <t>entry.588393791</t>
-  </si>
-  <si>
-    <t>entry.831172357</t>
-  </si>
-  <si>
-    <t>entry.2109138769</t>
+    <t>entry.98625466</t>
+  </si>
+  <si>
+    <t>entry.1289724168</t>
+  </si>
+  <si>
+    <t>entry.897012234</t>
+  </si>
+  <si>
+    <t>entry.1846392603</t>
+  </si>
+  <si>
+    <t>entry.1330307066</t>
+  </si>
+  <si>
+    <t>entry.1030855690</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,10 +138,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,21 +458,24 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -617,28 +605,28 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="1">
@@ -650,8 +638,8 @@
       <c r="L4" s="1">
         <v>0</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>26</v>
+      <c r="M4" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
3 sports registration added
</commit_message>
<xml_diff>
--- a/data/excel/register.xlsx
+++ b/data/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169F0FAA-F4CB-4055-A45F-D712CECB8D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8F6080-F4BA-40CC-BD60-629F57055F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>SportsName</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Team Name</t>
   </si>
   <si>
-    <t>Captian Name</t>
-  </si>
-  <si>
     <t>Full Name</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Payment UPI</t>
-  </si>
-  <si>
     <t>Contact Number</t>
   </si>
   <si>
@@ -90,13 +84,16 @@
     <t>entry.139421432</t>
   </si>
   <si>
-    <t>entry.1882846636</t>
-  </si>
-  <si>
     <t>Category </t>
   </si>
   <si>
     <t>ArmWrestling</t>
+  </si>
+  <si>
+    <t>Captain Name</t>
+  </si>
+  <si>
+    <t>UPI ID (payment proof)</t>
   </si>
 </sst>
 </file>
@@ -465,20 +462,17 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -489,25 +483,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
@@ -515,98 +509,98 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 sports backend updated
</commit_message>
<xml_diff>
--- a/data/excel/register.xlsx
+++ b/data/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8F6080-F4BA-40CC-BD60-629F57055F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB92F62-664A-4E56-A0D0-208A07BBD688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>SportsName</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Contact Number</t>
   </si>
   <si>
-    <t>Football </t>
-  </si>
-  <si>
-    <t>Cricket </t>
-  </si>
-  <si>
     <t>entry.1514101190</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>entry.139421432</t>
   </si>
   <si>
-    <t>Category </t>
-  </si>
-  <si>
     <t>ArmWrestling</t>
   </si>
   <si>
@@ -94,13 +85,37 @@
   </si>
   <si>
     <t>UPI ID (payment proof)</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/u/0/d/e/1FAIpQLScSKWrjiRruxbDUnELXAddEQw55am7JlyizTxYljnzwg7KWsQ/formResponse</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/u/0/d/e/1FAIpQLSf9-Q_vF_QVRrdXY9HXCF3eCeBwDA0olHFmglHlvaehmm6kkw/formResponse</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/u/0/d/e/1FAIpQLSdTDz8QcD_uvCC7TjIVf7GTRBaw-EX-jZG8UVXg-aamZSvGAw/formResponse</t>
+  </si>
+  <si>
+    <t>entry.370149229</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>Cricket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +127,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,12 +158,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -459,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C25FC1-1C7C-43BA-9684-6EC797E2D0F8}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,132 +503,144 @@
     <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Arm Wrestling Data
</commit_message>
<xml_diff>
--- a/data/excel/register.xlsx
+++ b/data/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun Kharkwal\OneDrive - Graphic Era University\Programmer's Space\Next js with Varun Kharkwal\03_OCTOBER_N\gehusports\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192B5AB9-75D9-4B3F-B684-D10494F8F655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCCB59A-1760-48DB-B17F-A2BA936266FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{249CFE40-A2DD-4BBF-88EE-17482A72F017}"/>
   </bookViews>
@@ -126,13 +126,13 @@
     <t>₹ 1500/- only</t>
   </si>
   <si>
-    <t>₹ 100/- for below 80 &amp; ₹ 150/- for above 80</t>
-  </si>
-  <si>
     <t>₹ 1000/- only</t>
   </si>
   <si>
     <t>https://cdn.discordapp.com/attachments/1162451241872412901/1169225366959837214/IMG-20231101-WA0018.jpg?ex=6554a0fa&amp;is=65422bfa&amp;hm=220a0402abcc6ca88f3ef35be5638ff9b15a071285d00af17bfde03f88461d07&amp;</t>
+  </si>
+  <si>
+    <t>₹ 50/- for all weight category</t>
   </si>
 </sst>
 </file>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C25FC1-1C7C-43BA-9684-6EC797E2D0F8}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +536,7 @@
     <col min="5" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5546875" customWidth="1"/>
     <col min="12" max="12" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -613,10 +613,10 @@
         <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>20</v>
@@ -654,7 +654,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>27</v>

</xml_diff>